<commit_message>
Further added models and implemented some textures.
</commit_message>
<xml_diff>
--- a/PostalFrog all files and docs/Asset list.xlsx
+++ b/PostalFrog all files and docs/Asset list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\PostalFrog all files and docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s210228\Documents\GitRepos\Postal-Frog\PostalFrog all files and docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06EA474-41A5-4816-A0BF-8F7799FDA319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B0F492-1A26-4D7D-A4A9-C6E9A817678E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3B1C447C-FF85-44DC-99E6-92DF2D0AA45D}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3B1C447C-FF85-44DC-99E6-92DF2D0AA45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
   <si>
     <t>Asset</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Leaves</t>
   </si>
   <si>
-    <t>house</t>
-  </si>
-  <si>
     <t>Border</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>simple exterior powerbox</t>
   </si>
   <si>
-    <t>white brick house with window and simple wood door</t>
-  </si>
-  <si>
     <t>Tiled slanted roof</t>
   </si>
   <si>
@@ -214,6 +208,21 @@
   </si>
   <si>
     <t>Tall Hedge module</t>
+  </si>
+  <si>
+    <t>HouseDoor</t>
+  </si>
+  <si>
+    <t>Simple wood door</t>
+  </si>
+  <si>
+    <t>white brick house with window and door</t>
+  </si>
+  <si>
+    <t>82 x 204 x 5</t>
+  </si>
+  <si>
+    <t>HouseWall</t>
   </si>
 </sst>
 </file>
@@ -568,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0774B79-99D7-4E20-8AF3-A469452CEFA3}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,10 +611,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -622,13 +631,13 @@
         <v>200</v>
       </c>
       <c r="E2">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -645,13 +654,13 @@
         <v>6</v>
       </c>
       <c r="E3">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,13 +677,13 @@
         <v>6</v>
       </c>
       <c r="E4">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -691,36 +700,36 @@
         <v>6</v>
       </c>
       <c r="E5">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>6</v>
       </c>
       <c r="E6">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -731,111 +740,111 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>40</v>
       </c>
       <c r="E7">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8">
         <v>24</v>
       </c>
       <c r="E8">
-        <v>512</v>
+        <v>2048</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9">
         <v>24</v>
       </c>
       <c r="E9">
-        <v>512</v>
+        <v>2048</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>42</v>
       </c>
       <c r="E10">
-        <v>512</v>
+        <v>2048</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>2048</v>
+      </c>
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-      <c r="E11">
-        <v>1024</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -852,13 +861,13 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <v>512</v>
+        <v>2048</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -875,13 +884,13 @@
         <v>20</v>
       </c>
       <c r="E13">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -898,24 +907,24 @@
         <v>6</v>
       </c>
       <c r="E14">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -924,56 +933,79 @@
         <v>1024</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16">
         <v>30</v>
       </c>
       <c r="E16">
-        <v>512</v>
+        <v>1024</v>
       </c>
       <c r="F16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17">
+        <v>2048</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18">
         <v>1024</v>
       </c>
-      <c r="F17" t="s">
-        <v>58</v>
-      </c>
-      <c r="G17" t="s">
-        <v>35</v>
+      <c r="F18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nearly all models but Frog complete added more textures
</commit_message>
<xml_diff>
--- a/PostalFrog all files and docs/Asset list.xlsx
+++ b/PostalFrog all files and docs/Asset list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s210228\Documents\GitRepos\Postal-Frog\PostalFrog all files and docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B0F492-1A26-4D7D-A4A9-C6E9A817678E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49425278-E91B-4B86-943A-8BA1D24BE711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3B1C447C-FF85-44DC-99E6-92DF2D0AA45D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>Asset</t>
   </si>
@@ -126,9 +126,6 @@
     <t>black box with white button</t>
   </si>
   <si>
-    <t>Hedge</t>
-  </si>
-  <si>
     <t>high/low poly?</t>
   </si>
   <si>
@@ -153,24 +150,12 @@
     <t>40 x 60 x 10</t>
   </si>
   <si>
-    <t>20 x 1 x 15</t>
-  </si>
-  <si>
     <t>Hedge leaf covered branch</t>
   </si>
   <si>
     <t>10 x 100 x 30</t>
   </si>
   <si>
-    <t>Fountain top</t>
-  </si>
-  <si>
-    <t>Fountain Bottom</t>
-  </si>
-  <si>
-    <t>Fountain centre</t>
-  </si>
-  <si>
     <t>Semicircular fountain basin, light stone</t>
   </si>
   <si>
@@ -183,9 +168,6 @@
     <t>150 x 20 x 300</t>
   </si>
   <si>
-    <t>20 x 250 x 20</t>
-  </si>
-  <si>
     <t>20 x 240 x 650</t>
   </si>
   <si>
@@ -223,16 +205,67 @@
   </si>
   <si>
     <t>HouseWall</t>
+  </si>
+  <si>
+    <t>FountainTop</t>
+  </si>
+  <si>
+    <t>FountainBottom</t>
+  </si>
+  <si>
+    <t>FountainCentre</t>
+  </si>
+  <si>
+    <t>40 x 250 x 20</t>
+  </si>
+  <si>
+    <t>30 x 1.5 x 22.5</t>
+  </si>
+  <si>
+    <t>HedgeModule</t>
+  </si>
+  <si>
+    <t>HedgeCorner</t>
+  </si>
+  <si>
+    <t>HedgeGate</t>
+  </si>
+  <si>
+    <t>Tall Hedge corner Module</t>
+  </si>
+  <si>
+    <t>Double width hedge module with an inset gate</t>
+  </si>
+  <si>
+    <t>100 x 300 x 10</t>
+  </si>
+  <si>
+    <t>100 x 300 x 100</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Grassy floor with a path from the gate to the door</t>
+  </si>
+  <si>
+    <t>420 x 2 x 890</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -577,17 +610,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0774B79-99D7-4E20-8AF3-A469452CEFA3}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -611,10 +644,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -634,10 +667,10 @@
         <v>2048</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -657,10 +690,10 @@
         <v>1024</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -680,10 +713,10 @@
         <v>1024</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -703,10 +736,10 @@
         <v>1024</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -726,10 +759,10 @@
         <v>1024</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,7 +773,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>40</v>
@@ -749,21 +782,21 @@
         <v>1024</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>24</v>
@@ -772,21 +805,21 @@
         <v>2048</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>24</v>
@@ -795,21 +828,21 @@
         <v>2048</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D10">
         <v>42</v>
@@ -818,21 +851,21 @@
         <v>2048</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -841,174 +874,244 @@
         <v>2048</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E12">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E13">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E14">
         <v>1024</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>1024</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>1024</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
       <c r="E17">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>2048</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>2048</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
+      </c>
+      <c r="E20">
+        <v>2048</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18">
-        <v>30</v>
-      </c>
-      <c r="E18">
-        <v>1024</v>
-      </c>
-      <c r="F18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" t="s">
-        <v>33</v>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>2048</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented more textures fixed door and doorbell models
</commit_message>
<xml_diff>
--- a/PostalFrog all files and docs/Asset list.xlsx
+++ b/PostalFrog all files and docs/Asset list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s210228\Documents\GitRepos\Postal-Frog\PostalFrog all files and docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49425278-E91B-4B86-943A-8BA1D24BE711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04645A45-5392-4DE8-A686-CF11E924B452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3B1C447C-FF85-44DC-99E6-92DF2D0AA45D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>Asset</t>
   </si>
@@ -183,9 +183,6 @@
     <t>700 x 150 x 150</t>
   </si>
   <si>
-    <t>2 x 6 x 1</t>
-  </si>
-  <si>
     <t>200 x 300 x 10</t>
   </si>
   <si>
@@ -250,6 +247,12 @@
   </si>
   <si>
     <t>420 x 2 x 890</t>
+  </si>
+  <si>
+    <t>actual polys</t>
+  </si>
+  <si>
+    <t>4 x 8 x 1</t>
   </si>
 </sst>
 </file>
@@ -610,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0774B79-99D7-4E20-8AF3-A469452CEFA3}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +630,7 @@
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -649,8 +652,11 @@
       <c r="G1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -673,7 +679,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -696,7 +702,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -719,7 +725,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -742,7 +748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -764,8 +770,11 @@
       <c r="G6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -782,15 +791,15 @@
         <v>1024</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -811,9 +820,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -834,9 +843,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -851,21 +860,21 @@
         <v>2048</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -880,15 +889,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12">
         <v>30</v>
@@ -897,13 +906,13 @@
         <v>1024</v>
       </c>
       <c r="F12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -926,7 +935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -949,7 +958,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -972,7 +981,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -995,7 +1004,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1012,21 +1021,24 @@
         <v>1024</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="G17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -1035,21 +1047,21 @@
         <v>2048</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19">
         <v>8</v>
@@ -1058,21 +1070,21 @@
         <v>2048</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20">
         <v>17</v>
@@ -1081,21 +1093,21 @@
         <v>2048</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21">
         <v>15</v>
@@ -1104,7 +1116,7 @@
         <v>2048</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G21" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Revert "functioning sounds,  missing water"
This reverts commit e443bbe57fabb86fba4ba96020cf90217bbfc0e1.
</commit_message>
<xml_diff>
--- a/PostalFrog all files and docs/Asset list.xlsx
+++ b/PostalFrog all files and docs/Asset list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s210228\Documents\GitRepos\Postal-Frog\PostalFrog all files and docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D28A46A-1FEA-4486-8F81-2C0DDDD35FC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04645A45-5392-4DE8-A686-CF11E924B452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3B1C447C-FF85-44DC-99E6-92DF2D0AA45D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>Asset</t>
   </si>
@@ -253,24 +253,6 @@
   </si>
   <si>
     <t>4 x 8 x 1</t>
-  </si>
-  <si>
-    <t>WindowBlinds</t>
-  </si>
-  <si>
-    <t>Romanblinds covering interior of window</t>
-  </si>
-  <si>
-    <t>230 x 130 x 5</t>
-  </si>
-  <si>
-    <t>PostalFrogLeap</t>
-  </si>
-  <si>
-    <t>Bull frog with post officer hat and bag leaping forward</t>
-  </si>
-  <si>
-    <t>10 x 3 x 5</t>
   </si>
 </sst>
 </file>
@@ -631,11 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0774B79-99D7-4E20-8AF3-A469452CEFA3}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I29" sqref="I29"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,42 +678,36 @@
       <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="I2">
-        <v>663</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3">
-        <v>200</v>
-      </c>
       <c r="E3">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3">
-        <v>832</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -744,18 +719,15 @@
         <v>1024</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
-      </c>
-      <c r="I4">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -770,24 +742,21 @@
         <v>1024</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -796,75 +765,69 @@
         <v>1024</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>
       </c>
       <c r="I6">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="E7">
         <v>1024</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
-        <v>38</v>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D8">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E8">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>40</v>
       </c>
       <c r="D9">
@@ -874,382 +837,293 @@
         <v>2048</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
-      </c>
-      <c r="I9">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="E10">
         <v>2048</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
       </c>
-      <c r="I10">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D11">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E11">
         <v>2048</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
         <v>31</v>
       </c>
-      <c r="I11">
-        <v>135</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
       </c>
       <c r="D12">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E12">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13">
-        <v>30</v>
-      </c>
       <c r="E13">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E14">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s">
         <v>32</v>
-      </c>
-      <c r="I14">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>1024</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
         <v>32</v>
-      </c>
-      <c r="I15">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>1024</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
         <v>32</v>
-      </c>
-      <c r="I16">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="D17">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="E17">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I17">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="G18" t="s">
         <v>32</v>
-      </c>
-      <c r="I18">
-        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="D19">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E20">
         <v>2048</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="G20" t="s">
         <v>32</v>
-      </c>
-      <c r="I20">
-        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E21">
         <v>2048</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G21" t="s">
         <v>32</v>
-      </c>
-      <c r="I21">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22">
-        <v>17</v>
-      </c>
-      <c r="E22">
-        <v>2048</v>
-      </c>
-      <c r="F22" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23">
-        <v>15</v>
-      </c>
-      <c r="E23">
-        <v>2048</v>
-      </c>
-      <c r="F23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" t="s">
-        <v>32</v>
-      </c>
-      <c r="I23">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
functioning sounds,  missing water
</commit_message>
<xml_diff>
--- a/PostalFrog all files and docs/Asset list.xlsx
+++ b/PostalFrog all files and docs/Asset list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s210228\Documents\GitRepos\Postal-Frog\PostalFrog all files and docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04645A45-5392-4DE8-A686-CF11E924B452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D28A46A-1FEA-4486-8F81-2C0DDDD35FC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3B1C447C-FF85-44DC-99E6-92DF2D0AA45D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="79">
   <si>
     <t>Asset</t>
   </si>
@@ -253,6 +253,24 @@
   </si>
   <si>
     <t>4 x 8 x 1</t>
+  </si>
+  <si>
+    <t>WindowBlinds</t>
+  </si>
+  <si>
+    <t>Romanblinds covering interior of window</t>
+  </si>
+  <si>
+    <t>230 x 130 x 5</t>
+  </si>
+  <si>
+    <t>PostalFrogLeap</t>
+  </si>
+  <si>
+    <t>Bull frog with post officer hat and bag leaping forward</t>
+  </si>
+  <si>
+    <t>10 x 3 x 5</t>
   </si>
 </sst>
 </file>
@@ -613,10 +631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0774B79-99D7-4E20-8AF3-A469452CEFA3}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,36 +697,42 @@
       <c r="G2" t="s">
         <v>31</v>
       </c>
+      <c r="I2">
+        <v>663</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="E3">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="I3">
+        <v>832</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -719,15 +744,18 @@
         <v>1024</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
         <v>32</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -742,21 +770,24 @@
         <v>1024</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
         <v>32</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -765,69 +796,75 @@
         <v>1024</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>
       </c>
       <c r="I6">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>1024</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="I7">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8">
         <v>40</v>
       </c>
-      <c r="D8">
-        <v>24</v>
-      </c>
       <c r="E8">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="I8">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D9">
@@ -837,293 +874,382 @@
         <v>2048</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
+      </c>
+      <c r="I9">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E10">
         <v>2048</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
       </c>
       <c r="D11">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E11">
         <v>2048</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="G11" t="s">
         <v>31</v>
       </c>
+      <c r="I11">
+        <v>135</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D12">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E12">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="I12">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E13">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="I13">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>2048</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14">
         <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-      <c r="E14">
-        <v>1024</v>
-      </c>
-      <c r="F14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>1024</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
         <v>32</v>
+      </c>
+      <c r="I15">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E16">
         <v>1024</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
         <v>32</v>
+      </c>
+      <c r="I16">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="D17">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E17">
-        <v>1024</v>
+        <v>2048</v>
       </c>
       <c r="F17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17">
-        <v>84</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
         <v>32</v>
+      </c>
+      <c r="I18">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E19">
-        <v>2048</v>
+        <v>1024</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G19" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="I19">
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D20">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E20">
         <v>2048</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G20" t="s">
         <v>32</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D21">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E21">
         <v>2048</v>
       </c>
       <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>2048</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>2048</v>
+      </c>
+      <c r="F23" t="s">
         <v>70</v>
       </c>
-      <c r="G21" t="s">
-        <v>32</v>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>